<commit_message>
Pva 1.09, Checklist PvA
+- PvA
+- Checklist PvA
</commit_message>
<xml_diff>
--- a/project_Documenten/checklist pva .xlsx
+++ b/project_Documenten/checklist pva .xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t xml:space="preserve">A Algemeen, lay-out en taalgebruik van het plan van aanpak </t>
   </si>
@@ -812,7 +812,7 @@
   <dimension ref="A2:C112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,7 +1358,9 @@
       <c r="A65" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="13"/>
+      <c r="B65" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C65">
         <v>1</v>
       </c>
@@ -1367,7 +1369,9 @@
       <c r="A66" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="13"/>
+      <c r="B66" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C66">
         <v>1</v>
       </c>
@@ -1376,7 +1380,9 @@
       <c r="A67" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="13"/>
+      <c r="B67" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C67">
         <v>1</v>
       </c>
@@ -1385,7 +1391,9 @@
       <c r="A68" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="13"/>
+      <c r="B68" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C68">
         <v>1</v>
       </c>
@@ -1404,7 +1412,9 @@
       <c r="A71" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B71" s="13"/>
+      <c r="B71" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C71">
         <v>1</v>
       </c>
@@ -1413,7 +1423,9 @@
       <c r="A72" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="13"/>
+      <c r="B72" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C72">
         <v>1</v>
       </c>
@@ -1422,7 +1434,9 @@
       <c r="A73" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="13"/>
+      <c r="B73" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C73">
         <v>1</v>
       </c>
@@ -1431,7 +1445,9 @@
       <c r="A74" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B74" s="13"/>
+      <c r="B74" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C74">
         <v>1</v>
       </c>
@@ -1440,7 +1456,9 @@
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="13"/>
+      <c r="B75" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C75">
         <v>1</v>
       </c>
@@ -1449,7 +1467,9 @@
       <c r="A76" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B76" s="13"/>
+      <c r="B76" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C76">
         <v>1</v>
       </c>
@@ -1458,7 +1478,9 @@
       <c r="A77" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B77" s="13"/>
+      <c r="B77" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C77">
         <v>1</v>
       </c>
@@ -1467,7 +1489,9 @@
       <c r="A78" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B78" s="13"/>
+      <c r="B78" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C78">
         <v>1</v>
       </c>
@@ -1550,7 +1574,9 @@
       <c r="A89" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B89" s="13"/>
+      <c r="B89" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C89">
         <v>1</v>
       </c>
@@ -1559,7 +1585,9 @@
       <c r="A90" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B90" s="13"/>
+      <c r="B90" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C90">
         <v>1</v>
       </c>
@@ -1568,7 +1596,9 @@
       <c r="A91" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B91" s="13"/>
+      <c r="B91" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C91">
         <v>1</v>
       </c>
@@ -1577,7 +1607,9 @@
       <c r="A92" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B92" s="13"/>
+      <c r="B92" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C92">
         <v>1</v>
       </c>
@@ -1586,7 +1618,9 @@
       <c r="A93" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B93" s="13"/>
+      <c r="B93" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C93">
         <v>1</v>
       </c>
@@ -1595,7 +1629,9 @@
       <c r="A94" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="13"/>
+      <c r="B94" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C94">
         <v>1</v>
       </c>
@@ -1604,7 +1640,9 @@
       <c r="A95" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B95" s="13"/>
+      <c r="B95" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C95">
         <v>1</v>
       </c>
@@ -1623,7 +1661,9 @@
       <c r="A98" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B98" s="13"/>
+      <c r="B98" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C98">
         <v>1</v>
       </c>
@@ -1632,7 +1672,9 @@
       <c r="A99" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B99" s="13"/>
+      <c r="B99" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C99">
         <v>1</v>
       </c>
@@ -1641,7 +1683,9 @@
       <c r="A100" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B100" s="13"/>
+      <c r="B100" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C100">
         <v>1</v>
       </c>
@@ -1660,7 +1704,9 @@
       <c r="A103" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B103" s="13"/>
+      <c r="B103" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C103">
         <v>1</v>
       </c>
@@ -1669,7 +1715,9 @@
       <c r="A104" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B104" s="13"/>
+      <c r="B104" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C104">
         <v>1</v>
       </c>
@@ -1678,7 +1726,9 @@
       <c r="A105" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B105" s="13"/>
+      <c r="B105" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C105">
         <v>1</v>
       </c>
@@ -1687,7 +1737,9 @@
       <c r="A106" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B106" s="13"/>
+      <c r="B106" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C106">
         <v>1</v>
       </c>
@@ -1696,7 +1748,9 @@
       <c r="A107" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B107" s="13"/>
+      <c r="B107" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="C107">
         <v>1</v>
       </c>
@@ -1715,7 +1769,9 @@
       <c r="A110" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B110" s="16"/>
+      <c r="B110" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="C110">
         <v>1</v>
       </c>
@@ -1786,6 +1842,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8428B090D81B34DA19517DD6F855647" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="461551752daf7baccd316804784cc5e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -1834,12 +1896,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1850,6 +1906,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AFAB33E-1031-49BA-A588-1C5301A99807}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F0A3F64-43C4-4516-B7CB-A76F5930C263}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1864,14 +1928,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AFAB33E-1031-49BA-A588-1C5301A99807}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC4B3EB1-E67D-4B64-B435-42996348D439}">
   <ds:schemaRefs>

</xml_diff>